<commit_message>
Se adiciona una HU en el S3 de MER
</commit_message>
<xml_diff>
--- a/documentacion/desarrollo/cronograma/Product Backlog Sibica.xlsx
+++ b/documentacion/desarrollo/cronograma/Product Backlog Sibica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeg76\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6B8C39-7841-4A14-B180-077767A26CF6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D364EB2-695C-4CC0-A854-F4A89CF6E865}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="SB6" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PB!$A$6:$I$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PB!$A$6:$I$60</definedName>
     <definedName name="_ftn1" localSheetId="1">PB!$C$17</definedName>
     <definedName name="_ftnref1" localSheetId="1">PB!$C$11</definedName>
   </definedNames>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="416">
   <si>
     <t>Enunciado de la Historia</t>
   </si>
@@ -3142,6 +3142,25 @@
       </rPr>
       <t>La plataforma ArcGis se encuentra caida</t>
     </r>
+  </si>
+  <si>
+    <t>RF26</t>
+  </si>
+  <si>
+    <t>HU054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Propuesta MER de los modulos de Sibica y Gestion de riesgos </t>
+  </si>
+  <si>
+    <t>Diego Castillo
+Ever Hidalo</t>
+  </si>
+  <si>
+    <t>Modelado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Propuesta MER de los modulos de Sibica y Panorama de riesgo de riesgos </t>
   </si>
 </sst>
 </file>
@@ -3450,7 +3469,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3654,6 +3673,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3663,9 +3685,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3673,6 +3692,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3719,6 +3741,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4051,11 +4079,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="95.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="74" t="s">
         <v>200</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -4150,8 +4178,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="A21" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="81.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4168,61 +4196,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
     </row>
     <row r="2" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="73"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
     </row>
     <row r="3" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="73"/>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
+      <c r="A3" s="74"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
     </row>
     <row r="4" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="73"/>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
+      <c r="A4" s="74"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
     </row>
     <row r="5" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="74"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
+      <c r="A5" s="75"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
     </row>
     <row r="6" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
@@ -5622,14 +5650,36 @@
       </c>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C60" s="3"/>
+    <row r="60" spans="1:9" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="23" t="s">
+        <v>410</v>
+      </c>
+      <c r="B60" s="49" t="s">
+        <v>411</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="D60" s="43" t="s">
+        <v>248</v>
+      </c>
+      <c r="E60" s="64" t="s">
+        <v>328</v>
+      </c>
+      <c r="F60" s="1"/>
+      <c r="G60" s="53">
+        <v>3</v>
+      </c>
+      <c r="H60" s="73" t="s">
+        <v>139</v>
+      </c>
+      <c r="I60" s="1"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C62" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A6:I59" xr:uid="{00000000-0009-0000-0000-000001000000}">
+  <autoFilter ref="A6:I60" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <filterColumn colId="6">
       <filters>
         <filter val="3"/>
@@ -5649,8 +5699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7139F943-C9B2-471B-9715-1F991D95FE77}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5663,18 +5713,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="76" t="s">
         <v>400</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="75"/>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
+      <c r="A2" s="76"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
     </row>
     <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -6040,51 +6090,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="74" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
     </row>
     <row r="2" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="73"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
     </row>
     <row r="3" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="73"/>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
+      <c r="A3" s="74"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
     </row>
     <row r="4" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="73"/>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
+      <c r="A4" s="74"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
     </row>
     <row r="5" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="74"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
+      <c r="A5" s="75"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
     </row>
     <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
@@ -6118,9 +6168,9 @@
         <v>5</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="76"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="77"/>
@@ -7402,6 +7452,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:G5"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="A24:A30"/>
+    <mergeCell ref="A32:A38"/>
+    <mergeCell ref="A48:A52"/>
+    <mergeCell ref="A54:A60"/>
+    <mergeCell ref="A62:A68"/>
+    <mergeCell ref="A118:A124"/>
     <mergeCell ref="A126:A132"/>
     <mergeCell ref="A40:A46"/>
     <mergeCell ref="A70:A76"/>
@@ -7410,16 +7470,6 @@
     <mergeCell ref="A94:A100"/>
     <mergeCell ref="A102:A108"/>
     <mergeCell ref="A110:A116"/>
-    <mergeCell ref="A32:A38"/>
-    <mergeCell ref="A48:A52"/>
-    <mergeCell ref="A54:A60"/>
-    <mergeCell ref="A62:A68"/>
-    <mergeCell ref="A118:A124"/>
-    <mergeCell ref="A1:G5"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="A24:A30"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7446,51 +7496,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="74" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
     </row>
     <row r="2" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="73"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
     </row>
     <row r="3" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="73"/>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
+      <c r="A3" s="74"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
     </row>
     <row r="4" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="73"/>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
+      <c r="A4" s="74"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
     </row>
     <row r="5" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="74"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
+      <c r="A5" s="75"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
     </row>
     <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
@@ -7524,11 +7574,11 @@
         <v>7</v>
       </c>
       <c r="D7" s="65"/>
-      <c r="E7" s="80" t="s">
+      <c r="E7" s="81" t="s">
         <v>397</v>
       </c>
-      <c r="F7" s="81"/>
-      <c r="G7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="83"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="77"/>
@@ -7650,9 +7700,9 @@
         <v>165</v>
       </c>
       <c r="D15" s="65"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="81"/>
-      <c r="G15" s="82"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="82"/>
+      <c r="G15" s="83"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="77"/>
@@ -7774,9 +7824,9 @@
         <v>178</v>
       </c>
       <c r="D23" s="65"/>
-      <c r="E23" s="80"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="82"/>
+      <c r="E23" s="81"/>
+      <c r="F23" s="82"/>
+      <c r="G23" s="83"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="17"/>
@@ -7857,9 +7907,9 @@
         <v>179</v>
       </c>
       <c r="D30" s="65"/>
-      <c r="E30" s="80"/>
-      <c r="F30" s="81"/>
-      <c r="G30" s="82"/>
+      <c r="E30" s="81"/>
+      <c r="F30" s="82"/>
+      <c r="G30" s="83"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="77"/>
@@ -7931,11 +7981,11 @@
         <v>180</v>
       </c>
       <c r="D36" s="6"/>
-      <c r="E36" s="83" t="s">
+      <c r="E36" s="84" t="s">
         <v>346</v>
       </c>
-      <c r="F36" s="84"/>
-      <c r="G36" s="85"/>
+      <c r="F36" s="85"/>
+      <c r="G36" s="86"/>
     </row>
     <row r="37" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="77"/>
@@ -8117,9 +8167,9 @@
         <v>181</v>
       </c>
       <c r="D52" s="6"/>
-      <c r="E52" s="86"/>
-      <c r="F52" s="87"/>
-      <c r="G52" s="88"/>
+      <c r="E52" s="87"/>
+      <c r="F52" s="88"/>
+      <c r="G52" s="89"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="77"/>
@@ -8200,11 +8250,11 @@
         <v>145</v>
       </c>
       <c r="D60" s="22"/>
-      <c r="E60" s="80" t="s">
+      <c r="E60" s="81" t="s">
         <v>351</v>
       </c>
-      <c r="F60" s="81"/>
-      <c r="G60" s="82"/>
+      <c r="F60" s="82"/>
+      <c r="G60" s="83"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="77"/>
@@ -8309,9 +8359,9 @@
         <v>164</v>
       </c>
       <c r="D68" s="65"/>
-      <c r="E68" s="80"/>
-      <c r="F68" s="81"/>
-      <c r="G68" s="82"/>
+      <c r="E68" s="81"/>
+      <c r="F68" s="82"/>
+      <c r="G68" s="83"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="77"/>
@@ -8390,11 +8440,11 @@
         <v>151</v>
       </c>
       <c r="D76" s="22"/>
-      <c r="E76" s="80" t="s">
+      <c r="E76" s="81" t="s">
         <v>348</v>
       </c>
-      <c r="F76" s="81"/>
-      <c r="G76" s="82"/>
+      <c r="F76" s="82"/>
+      <c r="G76" s="83"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" s="77"/>
@@ -8483,11 +8533,11 @@
         <v>141</v>
       </c>
       <c r="D84" s="6"/>
-      <c r="E84" s="80" t="s">
+      <c r="E84" s="81" t="s">
         <v>350</v>
       </c>
-      <c r="F84" s="81"/>
-      <c r="G84" s="82"/>
+      <c r="F84" s="82"/>
+      <c r="G84" s="83"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="77"/>
@@ -8570,6 +8620,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E52:G52"/>
     <mergeCell ref="A85:A91"/>
     <mergeCell ref="A16:A22"/>
     <mergeCell ref="A1:G5"/>
@@ -8586,11 +8641,6 @@
     <mergeCell ref="A53:A59"/>
     <mergeCell ref="A77:A83"/>
     <mergeCell ref="E68:G68"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E52:G52"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8600,10 +8650,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G102"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95:G95"/>
+    <sheetView topLeftCell="A80" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="81.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8617,51 +8667,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="74" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
     </row>
     <row r="2" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="73"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
     </row>
     <row r="3" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="73"/>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
+      <c r="A3" s="74"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
     </row>
     <row r="4" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="73"/>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
+      <c r="A4" s="74"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
     </row>
     <row r="5" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="74"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
+      <c r="A5" s="75"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
     </row>
     <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
@@ -8694,11 +8744,11 @@
         <v>136</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="80" t="s">
+      <c r="E7" s="81" t="s">
         <v>408</v>
       </c>
-      <c r="F7" s="81"/>
-      <c r="G7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="83"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="77"/>
@@ -8795,9 +8845,9 @@
         <v>144</v>
       </c>
       <c r="D15" s="22"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="81"/>
-      <c r="G15" s="82"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="82"/>
+      <c r="G15" s="83"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="77"/>
@@ -8886,9 +8936,9 @@
         <v>152</v>
       </c>
       <c r="D23" s="22"/>
-      <c r="E23" s="80"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="82"/>
+      <c r="E23" s="81"/>
+      <c r="F23" s="82"/>
+      <c r="G23" s="83"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="77"/>
@@ -8969,9 +9019,9 @@
         <v>153</v>
       </c>
       <c r="D31" s="22"/>
-      <c r="E31" s="80"/>
-      <c r="F31" s="81"/>
-      <c r="G31" s="82"/>
+      <c r="E31" s="81"/>
+      <c r="F31" s="82"/>
+      <c r="G31" s="83"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="77"/>
@@ -9068,9 +9118,9 @@
         <v>157</v>
       </c>
       <c r="D39" s="22"/>
-      <c r="E39" s="80"/>
-      <c r="F39" s="81"/>
-      <c r="G39" s="82"/>
+      <c r="E39" s="81"/>
+      <c r="F39" s="82"/>
+      <c r="G39" s="83"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="77"/>
@@ -9167,9 +9217,9 @@
         <v>156</v>
       </c>
       <c r="D47" s="22"/>
-      <c r="E47" s="80"/>
-      <c r="F47" s="81"/>
-      <c r="G47" s="82"/>
+      <c r="E47" s="81"/>
+      <c r="F47" s="82"/>
+      <c r="G47" s="83"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="77"/>
@@ -9282,9 +9332,9 @@
         <v>398</v>
       </c>
       <c r="D55" s="22"/>
-      <c r="E55" s="80"/>
-      <c r="F55" s="81"/>
-      <c r="G55" s="82"/>
+      <c r="E55" s="81"/>
+      <c r="F55" s="82"/>
+      <c r="G55" s="83"/>
     </row>
     <row r="56" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A56" s="77"/>
@@ -9367,9 +9417,9 @@
         <v>72</v>
       </c>
       <c r="D63" s="22"/>
-      <c r="E63" s="80"/>
-      <c r="F63" s="81"/>
-      <c r="G63" s="82"/>
+      <c r="E63" s="81"/>
+      <c r="F63" s="82"/>
+      <c r="G63" s="83"/>
     </row>
     <row r="64" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A64" s="77"/>
@@ -9450,9 +9500,9 @@
         <v>73</v>
       </c>
       <c r="D71" s="22"/>
-      <c r="E71" s="80"/>
-      <c r="F71" s="81"/>
-      <c r="G71" s="82"/>
+      <c r="E71" s="81"/>
+      <c r="F71" s="82"/>
+      <c r="G71" s="83"/>
     </row>
     <row r="72" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A72" s="77"/>
@@ -9543,9 +9593,9 @@
         <v>172</v>
       </c>
       <c r="D79" s="22"/>
-      <c r="E79" s="80"/>
-      <c r="F79" s="81"/>
-      <c r="G79" s="82"/>
+      <c r="E79" s="81"/>
+      <c r="F79" s="82"/>
+      <c r="G79" s="83"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" s="77"/>
@@ -9626,11 +9676,11 @@
         <v>87</v>
       </c>
       <c r="D87" s="60"/>
-      <c r="E87" s="80" t="s">
+      <c r="E87" s="81" t="s">
         <v>408</v>
       </c>
-      <c r="F87" s="81"/>
-      <c r="G87" s="82"/>
+      <c r="F87" s="82"/>
+      <c r="G87" s="83"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="77"/>
@@ -9711,11 +9761,11 @@
         <v>75</v>
       </c>
       <c r="D95" s="66"/>
-      <c r="E95" s="80" t="s">
+      <c r="E95" s="81" t="s">
         <v>408</v>
       </c>
-      <c r="F95" s="81"/>
-      <c r="G95" s="82"/>
+      <c r="F95" s="82"/>
+      <c r="G95" s="83"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" s="77"/>
@@ -9804,8 +9854,109 @@
       <c r="F102" s="10"/>
       <c r="G102" s="10"/>
     </row>
+    <row r="103" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="23" t="s">
+        <v>410</v>
+      </c>
+      <c r="B103" s="43"/>
+      <c r="C103" s="8" t="s">
+        <v>415</v>
+      </c>
+      <c r="D103" s="73"/>
+      <c r="E103" s="81"/>
+      <c r="F103" s="82"/>
+      <c r="G103" s="83"/>
+    </row>
+    <row r="104" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="77"/>
+      <c r="B104" s="73" t="s">
+        <v>115</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="D104" s="64" t="s">
+        <v>328</v>
+      </c>
+      <c r="E104" s="73" t="s">
+        <v>413</v>
+      </c>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A105" s="78"/>
+      <c r="B105" s="73"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="43"/>
+      <c r="E105" s="73"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A106" s="78"/>
+      <c r="B106" s="73"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="43"/>
+      <c r="E106" s="73"/>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A107" s="78"/>
+      <c r="B107" s="73"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="73"/>
+      <c r="E107" s="73"/>
+      <c r="F107" s="1"/>
+      <c r="G107" s="1"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A108" s="78"/>
+      <c r="B108" s="73"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="73"/>
+      <c r="E108" s="73"/>
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A109" s="78"/>
+      <c r="B109" s="73"/>
+      <c r="C109" s="1"/>
+      <c r="D109" s="73"/>
+      <c r="E109" s="73"/>
+      <c r="F109" s="1"/>
+      <c r="G109" s="1"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A110" s="79"/>
+      <c r="B110" s="10"/>
+      <c r="C110" s="10"/>
+      <c r="D110" s="10"/>
+      <c r="E110" s="10"/>
+      <c r="F110" s="10"/>
+      <c r="G110" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="27">
+    <mergeCell ref="E103:G103"/>
+    <mergeCell ref="A104:A110"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="A24:A30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="A32:A38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="A1:G5"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="A40:A46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="A56:A62"/>
     <mergeCell ref="E95:G95"/>
     <mergeCell ref="A96:A102"/>
     <mergeCell ref="A80:A86"/>
@@ -9816,21 +9967,6 @@
     <mergeCell ref="E79:G79"/>
     <mergeCell ref="E87:G87"/>
     <mergeCell ref="A88:A94"/>
-    <mergeCell ref="A40:A46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A1:G5"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="A24:A30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="A32:A38"/>
-    <mergeCell ref="E39:G39"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9842,8 +9978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:G22"/>
+    <sheetView topLeftCell="A15" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9855,51 +9991,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="74" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="73"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="73"/>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
+      <c r="A3" s="74"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="73"/>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
+      <c r="A4" s="74"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="74"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
+      <c r="A5" s="75"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
     </row>
     <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
@@ -9933,9 +10069,9 @@
         <v>142</v>
       </c>
       <c r="D7" s="43"/>
-      <c r="E7" s="89"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="91"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="91"/>
+      <c r="G7" s="92"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="77"/>
@@ -10020,20 +10156,20 @@
       <c r="A15" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="15" t="s">
         <v>76</v>
       </c>
       <c r="D15" s="22"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="81"/>
-      <c r="G15" s="82"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="82"/>
+      <c r="G15" s="83"/>
     </row>
     <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="77"/>
       <c r="B16" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="14" t="s">
         <v>242</v>
       </c>
       <c r="D16" s="35" t="s">
@@ -10050,7 +10186,7 @@
       <c r="B17" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="14" t="s">
         <v>243</v>
       </c>
       <c r="D17" s="35" t="s">
@@ -10067,7 +10203,7 @@
       <c r="B18" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="14" t="s">
         <v>244</v>
       </c>
       <c r="D18" s="35" t="s">
@@ -10082,7 +10218,7 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="78"/>
       <c r="B19" s="22"/>
-      <c r="C19" s="1"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
       <c r="F19" s="1"/>
@@ -10091,7 +10227,7 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="78"/>
       <c r="B20" s="22"/>
-      <c r="C20" s="1"/>
+      <c r="C20" s="14"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
       <c r="F20" s="1"/>
@@ -10100,7 +10236,7 @@
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="78"/>
       <c r="B21" s="22"/>
-      <c r="C21" s="1"/>
+      <c r="C21" s="14"/>
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
       <c r="F21" s="1"/>
@@ -10109,7 +10245,7 @@
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="79"/>
       <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
+      <c r="C22" s="42"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -10119,13 +10255,13 @@
       <c r="A23" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="15" t="s">
         <v>77</v>
       </c>
       <c r="D23" s="22"/>
-      <c r="E23" s="80"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="82"/>
+      <c r="E23" s="81"/>
+      <c r="F23" s="82"/>
+      <c r="G23" s="83"/>
     </row>
     <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="77"/>
@@ -10233,8 +10369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B6" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10246,51 +10382,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="74" t="s">
         <v>292</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="73"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="73"/>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
+      <c r="A3" s="74"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="73"/>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
+      <c r="A4" s="74"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="74"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
+      <c r="A5" s="75"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
     </row>
     <row r="6" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
@@ -10319,13 +10455,13 @@
       <c r="A7" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="96" t="s">
         <v>302</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="82"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="83"/>
     </row>
     <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="77"/>
@@ -10412,13 +10548,13 @@
         <v>158</v>
       </c>
       <c r="B15" s="44"/>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="96" t="s">
         <v>301</v>
       </c>
       <c r="D15" s="43"/>
-      <c r="E15" s="89"/>
-      <c r="F15" s="90"/>
-      <c r="G15" s="91"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="91"/>
+      <c r="G15" s="92"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="77"/>
@@ -10503,20 +10639,20 @@
       <c r="A23" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="15" t="s">
         <v>70</v>
       </c>
       <c r="D23" s="22"/>
-      <c r="E23" s="80"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="82"/>
+      <c r="E23" s="81"/>
+      <c r="F23" s="82"/>
+      <c r="G23" s="83"/>
     </row>
     <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="77"/>
       <c r="B24" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="14" t="s">
         <v>221</v>
       </c>
       <c r="D24" s="35" t="s">
@@ -10533,7 +10669,7 @@
       <c r="B25" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="14" t="s">
         <v>222</v>
       </c>
       <c r="D25" s="35" t="s">
@@ -10550,7 +10686,7 @@
       <c r="B26" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="14" t="s">
         <v>223</v>
       </c>
       <c r="D26" s="35" t="s">
@@ -10567,7 +10703,7 @@
       <c r="B27" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="14" t="s">
         <v>224</v>
       </c>
       <c r="D27" s="35" t="s">
@@ -10582,7 +10718,7 @@
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="78"/>
       <c r="B28" s="22"/>
-      <c r="C28" s="1"/>
+      <c r="C28" s="14"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
       <c r="F28" s="1"/>
@@ -10591,7 +10727,7 @@
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="78"/>
       <c r="B29" s="22"/>
-      <c r="C29" s="1"/>
+      <c r="C29" s="14"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
       <c r="F29" s="1"/>
@@ -10600,7 +10736,7 @@
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="79"/>
       <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
+      <c r="C30" s="42"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
@@ -10610,20 +10746,20 @@
       <c r="A31" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="15" t="s">
         <v>78</v>
       </c>
       <c r="D31" s="22"/>
-      <c r="E31" s="80"/>
-      <c r="F31" s="81"/>
-      <c r="G31" s="82"/>
+      <c r="E31" s="81"/>
+      <c r="F31" s="82"/>
+      <c r="G31" s="83"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="77"/>
       <c r="B32" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="14" t="s">
         <v>225</v>
       </c>
       <c r="D32" s="35" t="s">
@@ -10640,7 +10776,7 @@
       <c r="B33" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="14" t="s">
         <v>226</v>
       </c>
       <c r="D33" s="35" t="s">
@@ -10657,7 +10793,7 @@
       <c r="B34" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="14" t="s">
         <v>227</v>
       </c>
       <c r="D34" s="35" t="s">
@@ -10674,7 +10810,7 @@
       <c r="B35" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="14" t="s">
         <v>228</v>
       </c>
       <c r="D35" s="35" t="s">
@@ -10689,7 +10825,7 @@
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="78"/>
       <c r="B36" s="22"/>
-      <c r="C36" s="1"/>
+      <c r="C36" s="14"/>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
       <c r="F36" s="1"/>
@@ -10698,7 +10834,7 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="78"/>
       <c r="B37" s="22"/>
-      <c r="C37" s="1"/>
+      <c r="C37" s="14"/>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
       <c r="F37" s="1"/>
@@ -10707,7 +10843,7 @@
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="79"/>
       <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
+      <c r="C38" s="42"/>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -10717,20 +10853,20 @@
       <c r="A39" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="15" t="s">
         <v>79</v>
       </c>
       <c r="D39" s="22"/>
-      <c r="E39" s="80"/>
-      <c r="F39" s="81"/>
-      <c r="G39" s="82"/>
+      <c r="E39" s="81"/>
+      <c r="F39" s="82"/>
+      <c r="G39" s="83"/>
     </row>
     <row r="40" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="77"/>
       <c r="B40" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="14" t="s">
         <v>229</v>
       </c>
       <c r="D40" s="35" t="s">
@@ -10747,7 +10883,7 @@
       <c r="B41" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="14" t="s">
         <v>230</v>
       </c>
       <c r="D41" s="35" t="s">
@@ -10762,7 +10898,7 @@
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="78"/>
       <c r="B42" s="33"/>
-      <c r="C42" s="1"/>
+      <c r="C42" s="14"/>
       <c r="D42" s="22"/>
       <c r="E42" s="22"/>
       <c r="F42" s="1"/>
@@ -10771,7 +10907,7 @@
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="78"/>
       <c r="B43" s="33"/>
-      <c r="C43" s="1"/>
+      <c r="C43" s="14"/>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
       <c r="F43" s="1"/>
@@ -10780,7 +10916,7 @@
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="78"/>
       <c r="B44" s="22"/>
-      <c r="C44" s="1"/>
+      <c r="C44" s="14"/>
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
       <c r="F44" s="1"/>
@@ -10789,7 +10925,7 @@
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="78"/>
       <c r="B45" s="22"/>
-      <c r="C45" s="1"/>
+      <c r="C45" s="14"/>
       <c r="D45" s="22"/>
       <c r="E45" s="22"/>
       <c r="F45" s="1"/>
@@ -10798,7 +10934,7 @@
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="79"/>
       <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
+      <c r="C46" s="42"/>
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -10808,20 +10944,20 @@
       <c r="A47" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="15" t="s">
         <v>80</v>
       </c>
       <c r="D47" s="22"/>
-      <c r="E47" s="80"/>
-      <c r="F47" s="81"/>
-      <c r="G47" s="82"/>
+      <c r="E47" s="81"/>
+      <c r="F47" s="82"/>
+      <c r="G47" s="83"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="77"/>
       <c r="B48" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="14" t="s">
         <v>231</v>
       </c>
       <c r="D48" s="35" t="s">
@@ -10838,7 +10974,7 @@
       <c r="B49" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="14" t="s">
         <v>232</v>
       </c>
       <c r="D49" s="35" t="s">
@@ -10853,7 +10989,7 @@
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="78"/>
       <c r="B50" s="33"/>
-      <c r="C50" s="1"/>
+      <c r="C50" s="14"/>
       <c r="D50" s="22"/>
       <c r="E50" s="22"/>
       <c r="F50" s="1"/>
@@ -10862,7 +10998,7 @@
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="78"/>
       <c r="B51" s="33"/>
-      <c r="C51" s="1"/>
+      <c r="C51" s="14"/>
       <c r="D51" s="22"/>
       <c r="E51" s="22"/>
       <c r="F51" s="1"/>
@@ -10871,7 +11007,7 @@
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="78"/>
       <c r="B52" s="22"/>
-      <c r="C52" s="1"/>
+      <c r="C52" s="14"/>
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
       <c r="F52" s="1"/>
@@ -10880,7 +11016,7 @@
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="78"/>
       <c r="B53" s="22"/>
-      <c r="C53" s="1"/>
+      <c r="C53" s="14"/>
       <c r="D53" s="22"/>
       <c r="E53" s="22"/>
       <c r="F53" s="1"/>
@@ -10889,7 +11025,7 @@
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="79"/>
       <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
+      <c r="C54" s="42"/>
       <c r="D54" s="10"/>
       <c r="E54" s="10"/>
       <c r="F54" s="10"/>
@@ -10899,20 +11035,20 @@
       <c r="A55" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="15" t="s">
         <v>81</v>
       </c>
       <c r="D55" s="22"/>
-      <c r="E55" s="80"/>
-      <c r="F55" s="81"/>
-      <c r="G55" s="82"/>
+      <c r="E55" s="81"/>
+      <c r="F55" s="82"/>
+      <c r="G55" s="83"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="77"/>
       <c r="B56" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="C56" s="37" t="s">
+      <c r="C56" s="14" t="s">
         <v>286</v>
       </c>
       <c r="D56" s="36" t="s">
@@ -10929,7 +11065,7 @@
       <c r="B57" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="C57" s="37" t="s">
+      <c r="C57" s="14" t="s">
         <v>288</v>
       </c>
       <c r="D57" s="36" t="s">
@@ -10946,7 +11082,7 @@
       <c r="B58" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="C58" s="37" t="s">
+      <c r="C58" s="14" t="s">
         <v>289</v>
       </c>
       <c r="D58" s="36" t="s">
@@ -10961,7 +11097,7 @@
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="78"/>
       <c r="B59" s="33"/>
-      <c r="C59" s="1"/>
+      <c r="C59" s="14"/>
       <c r="D59" s="22"/>
       <c r="E59" s="22"/>
       <c r="F59" s="1"/>
@@ -10970,7 +11106,7 @@
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="78"/>
       <c r="B60" s="22"/>
-      <c r="C60" s="1"/>
+      <c r="C60" s="14"/>
       <c r="D60" s="22"/>
       <c r="E60" s="22"/>
       <c r="F60" s="1"/>
@@ -10979,7 +11115,7 @@
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="78"/>
       <c r="B61" s="22"/>
-      <c r="C61" s="1"/>
+      <c r="C61" s="14"/>
       <c r="D61" s="22"/>
       <c r="E61" s="22"/>
       <c r="F61" s="1"/>
@@ -10988,7 +11124,7 @@
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="79"/>
       <c r="B62" s="10"/>
-      <c r="C62" s="10"/>
+      <c r="C62" s="42"/>
       <c r="D62" s="10"/>
       <c r="E62" s="10"/>
       <c r="F62" s="10"/>
@@ -10998,13 +11134,13 @@
       <c r="A63" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="C63" s="8" t="s">
+      <c r="C63" s="15" t="s">
         <v>82</v>
       </c>
       <c r="D63" s="22"/>
-      <c r="E63" s="80"/>
-      <c r="F63" s="81"/>
-      <c r="G63" s="82"/>
+      <c r="E63" s="81"/>
+      <c r="F63" s="82"/>
+      <c r="G63" s="83"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="77"/>
@@ -11090,13 +11226,13 @@
         <v>171</v>
       </c>
       <c r="B71" s="44"/>
-      <c r="C71" s="15" t="s">
+      <c r="C71" s="8" t="s">
         <v>170</v>
       </c>
       <c r="D71" s="43"/>
-      <c r="E71" s="89"/>
-      <c r="F71" s="90"/>
-      <c r="G71" s="91"/>
+      <c r="E71" s="90"/>
+      <c r="F71" s="91"/>
+      <c r="G71" s="92"/>
     </row>
     <row r="72" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A72" s="77"/>
@@ -11179,6 +11315,16 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A1:G5"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="A24:A30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="A32:A38"/>
+    <mergeCell ref="E39:G39"/>
     <mergeCell ref="A72:A78"/>
     <mergeCell ref="E63:G63"/>
     <mergeCell ref="A64:A70"/>
@@ -11188,16 +11334,6 @@
     <mergeCell ref="A48:A54"/>
     <mergeCell ref="E55:G55"/>
     <mergeCell ref="A56:A62"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="A24:A30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="A32:A38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="A1:G5"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="A16:A22"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11209,8 +11345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11222,51 +11358,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="74" t="s">
         <v>295</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="73"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="73"/>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
+      <c r="A3" s="74"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="73"/>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
+      <c r="A4" s="74"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="74"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
+      <c r="A5" s="75"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
     </row>
     <row r="6" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
@@ -11296,20 +11432,20 @@
         <v>101</v>
       </c>
       <c r="B7"/>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="15" t="s">
         <v>74</v>
       </c>
       <c r="D7" s="22"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="82"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="83"/>
     </row>
     <row r="8" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="77"/>
       <c r="B8" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="14" t="s">
         <v>236</v>
       </c>
       <c r="D8" s="36" t="s">
@@ -11327,7 +11463,7 @@
       <c r="B9" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="14" t="s">
         <v>237</v>
       </c>
       <c r="D9" s="36" t="s">
@@ -11344,7 +11480,7 @@
       <c r="B10" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="14" t="s">
         <v>238</v>
       </c>
       <c r="D10" s="36" t="s">
@@ -11359,7 +11495,7 @@
     <row r="11" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="78"/>
       <c r="B11" s="22"/>
-      <c r="C11" s="1"/>
+      <c r="C11" s="14"/>
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
       <c r="F11" s="1"/>
@@ -11368,7 +11504,7 @@
     <row r="12" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="78"/>
       <c r="B12" s="22"/>
-      <c r="C12" s="1"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
       <c r="F12" s="1"/>
@@ -11377,7 +11513,7 @@
     <row r="13" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="78"/>
       <c r="B13" s="22"/>
-      <c r="C13" s="1"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
       <c r="F13" s="1"/>
@@ -11386,7 +11522,7 @@
     <row r="14" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="79"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
+      <c r="C14" s="42"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -11397,20 +11533,20 @@
         <v>282</v>
       </c>
       <c r="B15"/>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="15" t="s">
         <v>283</v>
       </c>
       <c r="D15" s="22"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="81"/>
-      <c r="G15" s="82"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="82"/>
+      <c r="G15" s="83"/>
     </row>
     <row r="16" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="77"/>
       <c r="B16" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="14" t="s">
         <v>284</v>
       </c>
       <c r="D16" s="36" t="s">
@@ -11427,7 +11563,7 @@
       <c r="B17" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="14" t="s">
         <v>285</v>
       </c>
       <c r="D17" s="36" t="s">
@@ -11442,7 +11578,7 @@
     <row r="18" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="78"/>
       <c r="B18" s="22"/>
-      <c r="C18" s="1"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
       <c r="F18" s="1"/>
@@ -11451,7 +11587,7 @@
     <row r="19" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="78"/>
       <c r="B19" s="22"/>
-      <c r="C19" s="1"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
       <c r="F19" s="1"/>
@@ -11460,7 +11596,7 @@
     <row r="20" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="78"/>
       <c r="B20" s="22"/>
-      <c r="C20" s="1"/>
+      <c r="C20" s="14"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
       <c r="F20" s="1"/>
@@ -11469,7 +11605,7 @@
     <row r="21" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="78"/>
       <c r="B21" s="22"/>
-      <c r="C21" s="1"/>
+      <c r="C21" s="14"/>
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
       <c r="F21" s="1"/>
@@ -11478,7 +11614,7 @@
     <row r="22" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="79"/>
       <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
+      <c r="C22" s="42"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -11492,12 +11628,12 @@
         <v>306</v>
       </c>
       <c r="D23" s="43"/>
-      <c r="E23" s="89"/>
-      <c r="F23" s="90"/>
-      <c r="G23" s="91"/>
+      <c r="E23" s="90"/>
+      <c r="F23" s="91"/>
+      <c r="G23" s="92"/>
     </row>
     <row r="24" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="92"/>
+      <c r="A24" s="93"/>
       <c r="B24" s="43"/>
       <c r="C24" s="14" t="s">
         <v>307</v>
@@ -11512,7 +11648,7 @@
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="93"/>
+      <c r="A25" s="94"/>
       <c r="B25" s="43"/>
       <c r="C25" s="14" t="s">
         <v>310</v>
@@ -11527,7 +11663,7 @@
       <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="93"/>
+      <c r="A26" s="94"/>
       <c r="B26" s="43"/>
       <c r="C26" s="14"/>
       <c r="D26" s="43"/>
@@ -11536,7 +11672,7 @@
       <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="93"/>
+      <c r="A27" s="94"/>
       <c r="B27" s="43"/>
       <c r="C27" s="14"/>
       <c r="D27" s="43"/>
@@ -11545,7 +11681,7 @@
       <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="93"/>
+      <c r="A28" s="94"/>
       <c r="B28" s="43"/>
       <c r="C28" s="14"/>
       <c r="D28" s="43"/>
@@ -11554,7 +11690,7 @@
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="93"/>
+      <c r="A29" s="94"/>
       <c r="B29" s="43"/>
       <c r="C29" s="14"/>
       <c r="D29" s="43"/>
@@ -11563,7 +11699,7 @@
       <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="94"/>
+      <c r="A30" s="95"/>
       <c r="B30" s="42"/>
       <c r="C30" s="42"/>
       <c r="D30" s="42"/>
@@ -11576,20 +11712,20 @@
         <v>11</v>
       </c>
       <c r="B31"/>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="14" t="s">
         <v>147</v>
       </c>
       <c r="D31" s="22"/>
-      <c r="E31" s="80"/>
-      <c r="F31" s="81"/>
-      <c r="G31" s="82"/>
+      <c r="E31" s="81"/>
+      <c r="F31" s="82"/>
+      <c r="G31" s="83"/>
     </row>
     <row r="32" spans="1:7" s="44" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="77"/>
       <c r="B32" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="14" t="s">
         <v>208</v>
       </c>
       <c r="D32" s="22" t="s">
@@ -11606,7 +11742,7 @@
       <c r="B33" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="14" t="s">
         <v>209</v>
       </c>
       <c r="D33" s="34" t="s">
@@ -11623,7 +11759,7 @@
       <c r="B34" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="14" t="s">
         <v>210</v>
       </c>
       <c r="D34" s="34" t="s">
@@ -11638,7 +11774,7 @@
     <row r="35" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="78"/>
       <c r="B35" s="22"/>
-      <c r="C35" s="1"/>
+      <c r="C35" s="14"/>
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
       <c r="F35" s="1"/>
@@ -11647,7 +11783,7 @@
     <row r="36" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="78"/>
       <c r="B36" s="22"/>
-      <c r="C36" s="1"/>
+      <c r="C36" s="14"/>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
       <c r="F36" s="1"/>
@@ -11656,7 +11792,7 @@
     <row r="37" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="78"/>
       <c r="B37" s="22"/>
-      <c r="C37" s="1"/>
+      <c r="C37" s="14"/>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
       <c r="F37" s="1"/>
@@ -11665,7 +11801,7 @@
     <row r="38" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="79"/>
       <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
+      <c r="C38" s="42"/>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -11676,20 +11812,20 @@
         <v>146</v>
       </c>
       <c r="B39"/>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="14" t="s">
         <v>148</v>
       </c>
       <c r="D39" s="22"/>
-      <c r="E39" s="80"/>
-      <c r="F39" s="81"/>
-      <c r="G39" s="82"/>
+      <c r="E39" s="81"/>
+      <c r="F39" s="82"/>
+      <c r="G39" s="83"/>
     </row>
     <row r="40" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="77"/>
       <c r="B40" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="C40" s="37" t="s">
+      <c r="C40" s="14" t="s">
         <v>265</v>
       </c>
       <c r="D40" s="35" t="s">
@@ -11706,7 +11842,7 @@
       <c r="B41" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="C41" s="37" t="s">
+      <c r="C41" s="14" t="s">
         <v>266</v>
       </c>
       <c r="D41" s="35" t="s">
@@ -11723,7 +11859,7 @@
       <c r="B42" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="44" t="s">
         <v>267</v>
       </c>
       <c r="D42" s="35" t="s">
@@ -11740,7 +11876,7 @@
       <c r="B43" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="C43" s="38" t="s">
+      <c r="C43" s="97" t="s">
         <v>268</v>
       </c>
       <c r="D43" s="35" t="s">
@@ -11755,7 +11891,7 @@
     <row r="44" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="78"/>
       <c r="B44" s="22"/>
-      <c r="C44" s="1"/>
+      <c r="C44" s="14"/>
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
       <c r="F44" s="1"/>
@@ -11764,7 +11900,7 @@
     <row r="45" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="78"/>
       <c r="B45" s="22"/>
-      <c r="C45" s="1"/>
+      <c r="C45" s="14"/>
       <c r="D45" s="22"/>
       <c r="E45" s="22"/>
       <c r="F45" s="1"/>
@@ -11773,7 +11909,7 @@
     <row r="46" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="79"/>
       <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
+      <c r="C46" s="42"/>
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -11784,16 +11920,16 @@
         <v>92</v>
       </c>
       <c r="B47" s="43"/>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="15" t="s">
         <v>83</v>
       </c>
       <c r="D47" s="43"/>
-      <c r="E47" s="89"/>
-      <c r="F47" s="90"/>
-      <c r="G47" s="91"/>
+      <c r="E47" s="90"/>
+      <c r="F47" s="91"/>
+      <c r="G47" s="92"/>
     </row>
     <row r="48" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="92"/>
+      <c r="A48" s="93"/>
       <c r="B48" s="43" t="s">
         <v>115</v>
       </c>
@@ -11804,7 +11940,7 @@
       <c r="G48" s="14"/>
     </row>
     <row r="49" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="93"/>
+      <c r="A49" s="94"/>
       <c r="B49" s="47" t="s">
         <v>116</v>
       </c>
@@ -11815,7 +11951,7 @@
       <c r="G49" s="14"/>
     </row>
     <row r="50" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="93"/>
+      <c r="A50" s="94"/>
       <c r="B50" s="47" t="s">
         <v>117</v>
       </c>
@@ -11826,7 +11962,7 @@
       <c r="G50" s="14"/>
     </row>
     <row r="51" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="93"/>
+      <c r="A51" s="94"/>
       <c r="B51" s="43" t="s">
         <v>118</v>
       </c>
@@ -11837,7 +11973,7 @@
       <c r="G51" s="14"/>
     </row>
     <row r="52" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="93"/>
+      <c r="A52" s="94"/>
       <c r="B52" s="43"/>
       <c r="C52" s="14"/>
       <c r="D52" s="43"/>
@@ -11846,7 +11982,7 @@
       <c r="G52" s="14"/>
     </row>
     <row r="53" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="93"/>
+      <c r="A53" s="94"/>
       <c r="B53" s="43"/>
       <c r="C53" s="14"/>
       <c r="D53" s="43"/>
@@ -11855,7 +11991,7 @@
       <c r="G53" s="14"/>
     </row>
     <row r="54" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="94"/>
+      <c r="A54" s="95"/>
       <c r="B54" s="42"/>
       <c r="C54" s="42"/>
       <c r="D54" s="42"/>
@@ -11868,16 +12004,16 @@
         <v>91</v>
       </c>
       <c r="B55" s="43"/>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="15" t="s">
         <v>84</v>
       </c>
       <c r="D55" s="43"/>
-      <c r="E55" s="89"/>
-      <c r="F55" s="90"/>
-      <c r="G55" s="91"/>
+      <c r="E55" s="90"/>
+      <c r="F55" s="91"/>
+      <c r="G55" s="92"/>
     </row>
     <row r="56" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="92"/>
+      <c r="A56" s="93"/>
       <c r="B56" s="43" t="s">
         <v>115</v>
       </c>
@@ -11888,7 +12024,7 @@
       <c r="G56" s="14"/>
     </row>
     <row r="57" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="93"/>
+      <c r="A57" s="94"/>
       <c r="B57" s="47" t="s">
         <v>116</v>
       </c>
@@ -11899,7 +12035,7 @@
       <c r="G57" s="14"/>
     </row>
     <row r="58" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="93"/>
+      <c r="A58" s="94"/>
       <c r="B58" s="47" t="s">
         <v>117</v>
       </c>
@@ -11910,7 +12046,7 @@
       <c r="G58" s="14"/>
     </row>
     <row r="59" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="93"/>
+      <c r="A59" s="94"/>
       <c r="B59" s="43" t="s">
         <v>118</v>
       </c>
@@ -11921,7 +12057,7 @@
       <c r="G59" s="14"/>
     </row>
     <row r="60" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="93"/>
+      <c r="A60" s="94"/>
       <c r="B60" s="43"/>
       <c r="C60" s="14"/>
       <c r="D60" s="43"/>
@@ -11930,7 +12066,7 @@
       <c r="G60" s="14"/>
     </row>
     <row r="61" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="93"/>
+      <c r="A61" s="94"/>
       <c r="B61" s="43"/>
       <c r="C61" s="14"/>
       <c r="D61" s="43"/>
@@ -11939,7 +12075,7 @@
       <c r="G61" s="14"/>
     </row>
     <row r="62" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="94"/>
+      <c r="A62" s="95"/>
       <c r="B62" s="42"/>
       <c r="C62" s="42"/>
       <c r="D62" s="42"/>
@@ -11952,16 +12088,16 @@
         <v>90</v>
       </c>
       <c r="B63" s="43"/>
-      <c r="C63" s="8" t="s">
+      <c r="C63" s="15" t="s">
         <v>85</v>
       </c>
       <c r="D63" s="43"/>
-      <c r="E63" s="89"/>
-      <c r="F63" s="90"/>
-      <c r="G63" s="91"/>
+      <c r="E63" s="90"/>
+      <c r="F63" s="91"/>
+      <c r="G63" s="92"/>
     </row>
     <row r="64" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="92"/>
+      <c r="A64" s="93"/>
       <c r="B64" s="43" t="s">
         <v>115</v>
       </c>
@@ -11972,7 +12108,7 @@
       <c r="G64" s="14"/>
     </row>
     <row r="65" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="93"/>
+      <c r="A65" s="94"/>
       <c r="B65" s="47" t="s">
         <v>116</v>
       </c>
@@ -11983,7 +12119,7 @@
       <c r="G65" s="14"/>
     </row>
     <row r="66" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="93"/>
+      <c r="A66" s="94"/>
       <c r="B66" s="47" t="s">
         <v>117</v>
       </c>
@@ -11994,7 +12130,7 @@
       <c r="G66" s="14"/>
     </row>
     <row r="67" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="93"/>
+      <c r="A67" s="94"/>
       <c r="B67" s="43" t="s">
         <v>118</v>
       </c>
@@ -12005,7 +12141,7 @@
       <c r="G67" s="14"/>
     </row>
     <row r="68" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="93"/>
+      <c r="A68" s="94"/>
       <c r="B68" s="43"/>
       <c r="C68" s="14"/>
       <c r="D68" s="43"/>
@@ -12014,7 +12150,7 @@
       <c r="G68" s="14"/>
     </row>
     <row r="69" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="93"/>
+      <c r="A69" s="94"/>
       <c r="B69" s="43"/>
       <c r="C69" s="14"/>
       <c r="D69" s="43"/>
@@ -12023,7 +12159,7 @@
       <c r="G69" s="14"/>
     </row>
     <row r="70" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="94"/>
+      <c r="A70" s="95"/>
       <c r="B70" s="42"/>
       <c r="C70" s="42"/>
       <c r="D70" s="42"/>
@@ -12035,12 +12171,12 @@
       <c r="A71" s="43"/>
       <c r="C71" s="15"/>
       <c r="D71" s="43"/>
-      <c r="E71" s="89"/>
-      <c r="F71" s="90"/>
-      <c r="G71" s="91"/>
+      <c r="E71" s="90"/>
+      <c r="F71" s="91"/>
+      <c r="G71" s="92"/>
     </row>
     <row r="72" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="92"/>
+      <c r="A72" s="93"/>
       <c r="B72" s="47"/>
       <c r="C72" s="14"/>
       <c r="D72" s="43"/>
@@ -12049,7 +12185,7 @@
       <c r="G72" s="14"/>
     </row>
     <row r="73" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="93"/>
+      <c r="A73" s="94"/>
       <c r="B73" s="47"/>
       <c r="C73" s="14"/>
       <c r="D73" s="43"/>
@@ -12058,7 +12194,7 @@
       <c r="G73" s="14"/>
     </row>
     <row r="74" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="93"/>
+      <c r="A74" s="94"/>
       <c r="B74" s="43"/>
       <c r="C74" s="14"/>
       <c r="D74" s="43"/>
@@ -12067,7 +12203,7 @@
       <c r="G74" s="14"/>
     </row>
     <row r="75" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="93"/>
+      <c r="A75" s="94"/>
       <c r="B75" s="43"/>
       <c r="C75" s="14"/>
       <c r="D75" s="43"/>
@@ -12076,7 +12212,7 @@
       <c r="G75" s="14"/>
     </row>
     <row r="76" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="93"/>
+      <c r="A76" s="94"/>
       <c r="B76" s="43"/>
       <c r="C76" s="14"/>
       <c r="D76" s="43"/>
@@ -12085,7 +12221,7 @@
       <c r="G76" s="14"/>
     </row>
     <row r="77" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="93"/>
+      <c r="A77" s="94"/>
       <c r="B77" s="43"/>
       <c r="C77" s="14"/>
       <c r="D77" s="43"/>
@@ -12094,7 +12230,7 @@
       <c r="G77" s="14"/>
     </row>
     <row r="78" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="94"/>
+      <c r="A78" s="95"/>
       <c r="B78" s="42"/>
       <c r="C78" s="42"/>
       <c r="D78" s="42"/>
@@ -12106,12 +12242,12 @@
       <c r="A79" s="43"/>
       <c r="C79" s="15"/>
       <c r="D79" s="43"/>
-      <c r="E79" s="89"/>
-      <c r="F79" s="90"/>
-      <c r="G79" s="91"/>
+      <c r="E79" s="90"/>
+      <c r="F79" s="91"/>
+      <c r="G79" s="92"/>
     </row>
     <row r="80" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="92"/>
+      <c r="A80" s="93"/>
       <c r="B80" s="43"/>
       <c r="C80" s="14"/>
       <c r="D80" s="43"/>
@@ -12120,7 +12256,7 @@
       <c r="G80" s="14"/>
     </row>
     <row r="81" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="93"/>
+      <c r="A81" s="94"/>
       <c r="B81" s="43"/>
       <c r="C81" s="14"/>
       <c r="D81" s="43"/>
@@ -12129,7 +12265,7 @@
       <c r="G81" s="14"/>
     </row>
     <row r="82" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="93"/>
+      <c r="A82" s="94"/>
       <c r="B82" s="43"/>
       <c r="C82" s="14"/>
       <c r="D82" s="43"/>
@@ -12138,7 +12274,7 @@
       <c r="G82" s="14"/>
     </row>
     <row r="83" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="93"/>
+      <c r="A83" s="94"/>
       <c r="B83" s="43"/>
       <c r="C83" s="14"/>
       <c r="D83" s="43"/>
@@ -12147,7 +12283,7 @@
       <c r="G83" s="14"/>
     </row>
     <row r="84" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="93"/>
+      <c r="A84" s="94"/>
       <c r="B84" s="43"/>
       <c r="C84" s="14"/>
       <c r="D84" s="43"/>
@@ -12156,7 +12292,7 @@
       <c r="G84" s="14"/>
     </row>
     <row r="85" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="93"/>
+      <c r="A85" s="94"/>
       <c r="B85" s="43"/>
       <c r="C85" s="14"/>
       <c r="D85" s="43"/>
@@ -12165,7 +12301,7 @@
       <c r="G85" s="14"/>
     </row>
     <row r="86" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="94"/>
+      <c r="A86" s="95"/>
       <c r="B86" s="42"/>
       <c r="C86" s="42"/>
       <c r="D86" s="42"/>
@@ -12177,12 +12313,12 @@
       <c r="A87" s="43"/>
       <c r="C87" s="15"/>
       <c r="D87" s="43"/>
-      <c r="E87" s="89"/>
-      <c r="F87" s="90"/>
-      <c r="G87" s="91"/>
+      <c r="E87" s="90"/>
+      <c r="F87" s="91"/>
+      <c r="G87" s="92"/>
     </row>
     <row r="88" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="92"/>
+      <c r="A88" s="93"/>
       <c r="B88" s="47"/>
       <c r="C88" s="14"/>
       <c r="D88" s="43"/>
@@ -12191,7 +12327,7 @@
       <c r="G88" s="14"/>
     </row>
     <row r="89" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="93"/>
+      <c r="A89" s="94"/>
       <c r="B89" s="47"/>
       <c r="C89" s="14"/>
       <c r="D89" s="43"/>
@@ -12200,7 +12336,7 @@
       <c r="G89" s="14"/>
     </row>
     <row r="90" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="93"/>
+      <c r="A90" s="94"/>
       <c r="B90" s="43"/>
       <c r="C90" s="14"/>
       <c r="D90" s="43"/>
@@ -12209,7 +12345,7 @@
       <c r="G90" s="14"/>
     </row>
     <row r="91" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="93"/>
+      <c r="A91" s="94"/>
       <c r="B91" s="43"/>
       <c r="C91" s="14"/>
       <c r="D91" s="43"/>
@@ -12218,7 +12354,7 @@
       <c r="G91" s="14"/>
     </row>
     <row r="92" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="93"/>
+      <c r="A92" s="94"/>
       <c r="B92" s="43"/>
       <c r="C92" s="14"/>
       <c r="D92" s="43"/>
@@ -12227,7 +12363,7 @@
       <c r="G92" s="14"/>
     </row>
     <row r="93" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="93"/>
+      <c r="A93" s="94"/>
       <c r="B93" s="43"/>
       <c r="C93" s="14"/>
       <c r="D93" s="43"/>
@@ -12236,7 +12372,7 @@
       <c r="G93" s="14"/>
     </row>
     <row r="94" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="94"/>
+      <c r="A94" s="95"/>
       <c r="B94" s="42"/>
       <c r="C94" s="42"/>
       <c r="D94" s="42"/>
@@ -12248,12 +12384,12 @@
       <c r="A95" s="43"/>
       <c r="C95" s="15"/>
       <c r="D95" s="43"/>
-      <c r="E95" s="89"/>
-      <c r="F95" s="90"/>
-      <c r="G95" s="91"/>
+      <c r="E95" s="90"/>
+      <c r="F95" s="91"/>
+      <c r="G95" s="92"/>
     </row>
     <row r="96" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="92"/>
+      <c r="A96" s="93"/>
       <c r="B96" s="43"/>
       <c r="C96" s="14"/>
       <c r="D96" s="43"/>
@@ -12262,7 +12398,7 @@
       <c r="G96" s="14"/>
     </row>
     <row r="97" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="93"/>
+      <c r="A97" s="94"/>
       <c r="B97" s="43"/>
       <c r="C97" s="14"/>
       <c r="D97" s="43"/>
@@ -12271,7 +12407,7 @@
       <c r="G97" s="14"/>
     </row>
     <row r="98" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="93"/>
+      <c r="A98" s="94"/>
       <c r="B98" s="43"/>
       <c r="C98" s="14"/>
       <c r="D98" s="43"/>
@@ -12280,7 +12416,7 @@
       <c r="G98" s="14"/>
     </row>
     <row r="99" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="93"/>
+      <c r="A99" s="94"/>
       <c r="B99" s="43"/>
       <c r="C99" s="14"/>
       <c r="D99" s="43"/>
@@ -12289,7 +12425,7 @@
       <c r="G99" s="14"/>
     </row>
     <row r="100" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="93"/>
+      <c r="A100" s="94"/>
       <c r="B100" s="43"/>
       <c r="C100" s="14"/>
       <c r="D100" s="43"/>
@@ -12298,7 +12434,7 @@
       <c r="G100" s="14"/>
     </row>
     <row r="101" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="93"/>
+      <c r="A101" s="94"/>
       <c r="B101" s="43"/>
       <c r="C101" s="14"/>
       <c r="D101" s="43"/>
@@ -12307,7 +12443,7 @@
       <c r="G101" s="14"/>
     </row>
     <row r="102" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="94"/>
+      <c r="A102" s="95"/>
       <c r="B102" s="42"/>
       <c r="C102" s="42"/>
       <c r="D102" s="42"/>
@@ -12319,12 +12455,12 @@
       <c r="A103" s="43"/>
       <c r="C103" s="15"/>
       <c r="D103" s="43"/>
-      <c r="E103" s="89"/>
-      <c r="F103" s="90"/>
-      <c r="G103" s="91"/>
+      <c r="E103" s="90"/>
+      <c r="F103" s="91"/>
+      <c r="G103" s="92"/>
     </row>
     <row r="104" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="92"/>
+      <c r="A104" s="93"/>
       <c r="B104" s="43"/>
       <c r="C104" s="14"/>
       <c r="D104" s="43"/>
@@ -12333,7 +12469,7 @@
       <c r="G104" s="14"/>
     </row>
     <row r="105" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="93"/>
+      <c r="A105" s="94"/>
       <c r="B105" s="43"/>
       <c r="C105" s="14"/>
       <c r="D105" s="43"/>
@@ -12342,7 +12478,7 @@
       <c r="G105" s="14"/>
     </row>
     <row r="106" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="93"/>
+      <c r="A106" s="94"/>
       <c r="B106" s="43"/>
       <c r="C106" s="14"/>
       <c r="D106" s="43"/>
@@ -12351,7 +12487,7 @@
       <c r="G106" s="14"/>
     </row>
     <row r="107" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="93"/>
+      <c r="A107" s="94"/>
       <c r="B107" s="43"/>
       <c r="C107" s="14"/>
       <c r="D107" s="43"/>
@@ -12360,7 +12496,7 @@
       <c r="G107" s="14"/>
     </row>
     <row r="108" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="93"/>
+      <c r="A108" s="94"/>
       <c r="B108" s="43"/>
       <c r="C108" s="14"/>
       <c r="D108" s="43"/>
@@ -12369,7 +12505,7 @@
       <c r="G108" s="14"/>
     </row>
     <row r="109" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="93"/>
+      <c r="A109" s="94"/>
       <c r="B109" s="43"/>
       <c r="C109" s="14"/>
       <c r="D109" s="43"/>
@@ -12378,7 +12514,7 @@
       <c r="G109" s="14"/>
     </row>
     <row r="110" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="94"/>
+      <c r="A110" s="95"/>
       <c r="B110" s="42"/>
       <c r="C110" s="42"/>
       <c r="D110" s="42"/>
@@ -12388,15 +12524,12 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A96:A102"/>
-    <mergeCell ref="E103:G103"/>
-    <mergeCell ref="A104:A110"/>
-    <mergeCell ref="A72:A78"/>
-    <mergeCell ref="E79:G79"/>
-    <mergeCell ref="A80:A86"/>
-    <mergeCell ref="E87:G87"/>
-    <mergeCell ref="A88:A94"/>
-    <mergeCell ref="E95:G95"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="A1:G5"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="A16:A22"/>
     <mergeCell ref="E71:G71"/>
     <mergeCell ref="A24:A30"/>
     <mergeCell ref="E31:G31"/>
@@ -12409,12 +12542,15 @@
     <mergeCell ref="A56:A62"/>
     <mergeCell ref="E63:G63"/>
     <mergeCell ref="A64:A70"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="A1:G5"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="A96:A102"/>
+    <mergeCell ref="E103:G103"/>
+    <mergeCell ref="A104:A110"/>
+    <mergeCell ref="A72:A78"/>
+    <mergeCell ref="E79:G79"/>
+    <mergeCell ref="A80:A86"/>
+    <mergeCell ref="E87:G87"/>
+    <mergeCell ref="A88:A94"/>
+    <mergeCell ref="E95:G95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
se consolida el ajuste del s4
</commit_message>
<xml_diff>
--- a/documentacion/desarrollo/cronograma/Product Backlog Sibica.xlsx
+++ b/documentacion/desarrollo/cronograma/Product Backlog Sibica.xlsx
@@ -14631,10 +14631,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView topLeftCell="A56" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15359,10 +15359,212 @@
       <c r="F62" s="41"/>
       <c r="G62" s="41"/>
     </row>
+    <row r="63" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A63" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D63" s="21"/>
+      <c r="E63" s="90"/>
+      <c r="F63" s="91"/>
+      <c r="G63" s="92"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="86"/>
+      <c r="B64" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="D64" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="E64" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="87"/>
+      <c r="B65" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="D65" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="E65" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="87"/>
+      <c r="B66" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C66" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="D66" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="E66" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="87"/>
+      <c r="B67" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C67" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="D67" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="E67" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="87"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="21"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="87"/>
+      <c r="B69" s="21"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="88"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="41"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
+    </row>
+    <row r="71" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A71" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D71" s="21"/>
+      <c r="E71" s="90"/>
+      <c r="F71" s="91"/>
+      <c r="G71" s="92"/>
+    </row>
+    <row r="72" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="86"/>
+      <c r="B72" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="C72" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="D72" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="E72" s="34" t="s">
+        <v>296</v>
+      </c>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+    </row>
+    <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="87"/>
+      <c r="B73" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="D73" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="E73" s="34" t="s">
+        <v>296</v>
+      </c>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="87"/>
+      <c r="B74" s="32"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="21"/>
+      <c r="E74" s="21"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="87"/>
+      <c r="B75" s="32"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="21"/>
+      <c r="E75" s="21"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="87"/>
+      <c r="B76" s="21"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="21"/>
+      <c r="E76" s="21"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="87"/>
+      <c r="B77" s="21"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="21"/>
+      <c r="E77" s="21"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="88"/>
+      <c r="B78" s="9"/>
+      <c r="C78" s="41"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="19">
+    <mergeCell ref="A64:A70"/>
+    <mergeCell ref="E71:G71"/>
+    <mergeCell ref="A72:A78"/>
     <mergeCell ref="E55:G55"/>
     <mergeCell ref="A56:A62"/>
+    <mergeCell ref="E63:G63"/>
     <mergeCell ref="E47:G47"/>
     <mergeCell ref="A48:A54"/>
     <mergeCell ref="E31:G31"/>
@@ -15386,8 +15588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15759,12 +15961,12 @@
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
     </row>
-    <row r="31" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
-        <v>93</v>
+        <v>282</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>78</v>
+        <v>283</v>
       </c>
       <c r="D31" s="21"/>
       <c r="E31" s="90"/>
@@ -15773,69 +15975,53 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="86"/>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="38" t="s">
         <v>115</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="D32" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="E32" s="34" t="s">
-        <v>303</v>
+        <v>284</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>287</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>304</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="87"/>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="38" t="s">
         <v>116</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="D33" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="E33" s="34" t="s">
-        <v>303</v>
+        <v>285</v>
+      </c>
+      <c r="D33" s="35" t="s">
+        <v>287</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>304</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="87"/>
-      <c r="B34" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="D34" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="E34" s="34" t="s">
-        <v>303</v>
-      </c>
+      <c r="B34" s="21"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="87"/>
-      <c r="B35" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="D35" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="E35" s="34" t="s">
-        <v>303</v>
-      </c>
+      <c r="B35" s="21"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
@@ -15866,188 +16052,6 @@
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
     </row>
-    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D39" s="21"/>
-      <c r="E39" s="90"/>
-      <c r="F39" s="91"/>
-      <c r="G39" s="92"/>
-    </row>
-    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="86"/>
-      <c r="B40" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="D40" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="E40" s="34" t="s">
-        <v>296</v>
-      </c>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="87"/>
-      <c r="B41" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="D41" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="E41" s="34" t="s">
-        <v>296</v>
-      </c>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="87"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="87"/>
-      <c r="B43" s="32"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="87"/>
-      <c r="B44" s="21"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="87"/>
-      <c r="B45" s="21"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="88"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="41"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-    </row>
-    <row r="47" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A47" s="24" t="s">
-        <v>282</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="D47" s="21"/>
-      <c r="E47" s="90"/>
-      <c r="F47" s="91"/>
-      <c r="G47" s="92"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="86"/>
-      <c r="B48" s="38" t="s">
-        <v>115</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="D48" s="35" t="s">
-        <v>287</v>
-      </c>
-      <c r="E48" s="21" t="s">
-        <v>304</v>
-      </c>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="87"/>
-      <c r="B49" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="D49" s="35" t="s">
-        <v>287</v>
-      </c>
-      <c r="E49" s="21" t="s">
-        <v>304</v>
-      </c>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="87"/>
-      <c r="B50" s="21"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="87"/>
-      <c r="B51" s="21"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="87"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="87"/>
-      <c r="B53" s="21"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="88"/>
-      <c r="B54" s="9"/>
-      <c r="C54" s="41"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-    </row>
     <row r="79" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A79" s="105" t="s">
         <v>103</v>
@@ -16148,7 +16152,7 @@
       <c r="G86" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="11">
     <mergeCell ref="E79:G79"/>
     <mergeCell ref="A80:A86"/>
     <mergeCell ref="A1:G5"/>
@@ -16160,10 +16164,6 @@
     <mergeCell ref="A24:A30"/>
     <mergeCell ref="E31:G31"/>
     <mergeCell ref="A32:A38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="A40:A46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="A48:A54"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16175,8 +16175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:C39"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
se agrega estado a algunos pendientes
</commit_message>
<xml_diff>
--- a/documentacion/desarrollo/cronograma/Product Backlog Sibica.xlsx
+++ b/documentacion/desarrollo/cronograma/Product Backlog Sibica.xlsx
@@ -27,6 +27,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PB!$A$6:$I$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Pendientes!$A$1:$F$60</definedName>
     <definedName name="_ftn1" localSheetId="1">PB!$C$17</definedName>
     <definedName name="_ftnref1" localSheetId="1">PB!$C$11</definedName>
   </definedNames>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1641" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1643" uniqueCount="633">
   <si>
     <t>Enunciado de la Historia</t>
   </si>
@@ -3806,6 +3807,9 @@
   </si>
   <si>
     <t>Al momento de guardar un tipo de amoclamiento, muestra mensaje de error</t>
+  </si>
+  <si>
+    <t>se le envia correo a wilmar para que habilite los permisos</t>
   </si>
 </sst>
 </file>
@@ -4158,7 +4162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4502,6 +4506,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8691,25 +8698,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="125" t="s">
         <v>612</v>
       </c>
-      <c r="B1" s="124" t="s">
+      <c r="B1" s="125" t="s">
         <v>613</v>
       </c>
-      <c r="C1" s="124" t="s">
+      <c r="C1" s="125" t="s">
         <v>614</v>
       </c>
-      <c r="D1" s="124" t="s">
+      <c r="D1" s="125" t="s">
         <v>615</v>
       </c>
-      <c r="E1" s="124" t="s">
+      <c r="E1" s="125" t="s">
         <v>616</v>
       </c>
-      <c r="F1" s="124" t="s">
+      <c r="F1" s="125" t="s">
         <v>617</v>
       </c>
-      <c r="G1" s="124" t="s">
+      <c r="G1" s="125" t="s">
         <v>618</v>
       </c>
     </row>
@@ -8717,19 +8724,19 @@
       <c r="A2" s="122">
         <v>1</v>
       </c>
-      <c r="B2" s="125" t="s">
+      <c r="B2" s="126" t="s">
         <v>619</v>
       </c>
-      <c r="C2" s="123">
+      <c r="C2" s="124">
         <v>43734</v>
       </c>
-      <c r="D2" s="123">
+      <c r="D2" s="124">
         <v>43736</v>
       </c>
       <c r="E2" s="122" t="s">
         <v>620</v>
       </c>
-      <c r="F2" s="126" t="s">
+      <c r="F2" s="127" t="s">
         <v>621</v>
       </c>
       <c r="G2" s="122"/>
@@ -8741,7 +8748,7 @@
       <c r="B3" s="122" t="s">
         <v>622</v>
       </c>
-      <c r="C3" s="123">
+      <c r="C3" s="124">
         <v>43734</v>
       </c>
       <c r="D3" s="122"/>
@@ -8760,7 +8767,7 @@
       <c r="B4" s="122" t="s">
         <v>624</v>
       </c>
-      <c r="C4" s="123">
+      <c r="C4" s="124">
         <v>43734</v>
       </c>
       <c r="D4" s="122"/>
@@ -8779,16 +8786,16 @@
       <c r="B5" s="122" t="s">
         <v>625</v>
       </c>
-      <c r="C5" s="123">
+      <c r="C5" s="124">
         <v>43734</v>
       </c>
-      <c r="D5" s="123">
+      <c r="D5" s="124">
         <v>43736</v>
       </c>
       <c r="E5" s="122" t="s">
         <v>620</v>
       </c>
-      <c r="F5" s="126" t="s">
+      <c r="F5" s="127" t="s">
         <v>621</v>
       </c>
       <c r="G5" s="122"/>
@@ -8800,7 +8807,7 @@
       <c r="B6" s="122" t="s">
         <v>626</v>
       </c>
-      <c r="C6" s="123">
+      <c r="C6" s="124">
         <v>43734</v>
       </c>
       <c r="D6" s="122"/>
@@ -8819,16 +8826,16 @@
       <c r="B7" s="122" t="s">
         <v>628</v>
       </c>
-      <c r="C7" s="123">
+      <c r="C7" s="124">
         <v>43734</v>
       </c>
-      <c r="D7" s="123">
+      <c r="D7" s="124">
         <v>43736</v>
       </c>
       <c r="E7" s="122" t="s">
         <v>627</v>
       </c>
-      <c r="F7" s="126" t="s">
+      <c r="F7" s="127" t="s">
         <v>621</v>
       </c>
       <c r="G7" s="122"/>
@@ -8840,7 +8847,7 @@
       <c r="B8" s="122" t="s">
         <v>629</v>
       </c>
-      <c r="C8" s="123">
+      <c r="C8" s="124">
         <v>43734</v>
       </c>
       <c r="D8" s="122"/>
@@ -8859,7 +8866,7 @@
       <c r="B9" s="122" t="s">
         <v>630</v>
       </c>
-      <c r="C9" s="123">
+      <c r="C9" s="124">
         <v>43737</v>
       </c>
       <c r="D9" s="122"/>
@@ -8878,7 +8885,7 @@
       <c r="B10" s="122" t="s">
         <v>631</v>
       </c>
-      <c r="C10" s="123">
+      <c r="C10" s="124">
         <v>43737</v>
       </c>
       <c r="D10" s="122"/>
@@ -11307,10 +11314,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B30" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11332,7 +11340,7 @@
       <c r="E1" s="102"/>
       <c r="F1" s="102"/>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="82"/>
       <c r="B2" s="82"/>
       <c r="C2" s="82"/>
@@ -11340,7 +11348,7 @@
       <c r="E2" s="102"/>
       <c r="F2" s="102"/>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="103" t="s">
         <v>400</v>
       </c>
@@ -11360,7 +11368,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="112" t="s">
         <v>362</v>
       </c>
@@ -11378,7 +11386,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="112" t="s">
         <v>363</v>
       </c>
@@ -11394,7 +11402,7 @@
       <c r="E5" s="105"/>
       <c r="F5" s="119"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="112" t="s">
         <v>364</v>
       </c>
@@ -11412,7 +11420,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="112" t="s">
         <v>365</v>
       </c>
@@ -11430,7 +11438,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="112" t="s">
         <v>366</v>
       </c>
@@ -11446,7 +11454,7 @@
       <c r="E8" s="105"/>
       <c r="F8" s="119"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="112" t="s">
         <v>367</v>
       </c>
@@ -11464,7 +11472,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="112" t="s">
         <v>368</v>
       </c>
@@ -11480,7 +11488,7 @@
       <c r="E10" s="105"/>
       <c r="F10" s="119"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="112" t="s">
         <v>369</v>
       </c>
@@ -11498,7 +11506,7 @@
       </c>
       <c r="F11" s="119"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="112" t="s">
         <v>370</v>
       </c>
@@ -11524,13 +11532,15 @@
       <c r="C13" s="114" t="s">
         <v>373</v>
       </c>
-      <c r="D13" s="104" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" s="105"/>
+      <c r="D13" s="123" t="s">
+        <v>327</v>
+      </c>
+      <c r="E13" s="105" t="s">
+        <v>611</v>
+      </c>
       <c r="F13" s="119"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="112" t="s">
         <v>372</v>
       </c>
@@ -11544,7 +11554,7 @@
       </c>
       <c r="F14" s="119"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="112" t="s">
         <v>384</v>
       </c>
@@ -11562,7 +11572,7 @@
       </c>
       <c r="F15" s="119"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="112" t="s">
         <v>385</v>
       </c>
@@ -11576,7 +11586,7 @@
       </c>
       <c r="F16" s="119"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="112" t="s">
         <v>386</v>
       </c>
@@ -11594,7 +11604,7 @@
       </c>
       <c r="F17" s="119"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="112" t="s">
         <v>387</v>
       </c>
@@ -11612,7 +11622,7 @@
       </c>
       <c r="F18" s="119"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="112" t="s">
         <v>388</v>
       </c>
@@ -11628,7 +11638,7 @@
       <c r="E19" s="105"/>
       <c r="F19" s="119"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="112" t="s">
         <v>389</v>
       </c>
@@ -11644,7 +11654,7 @@
       <c r="E20" s="105"/>
       <c r="F20" s="119"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="112" t="s">
         <v>390</v>
       </c>
@@ -11660,7 +11670,7 @@
       <c r="E21" s="105"/>
       <c r="F21" s="119"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="112" t="s">
         <v>391</v>
       </c>
@@ -11676,7 +11686,7 @@
       <c r="E22" s="105"/>
       <c r="F22" s="119"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="112" t="s">
         <v>392</v>
       </c>
@@ -11710,7 +11720,7 @@
       </c>
       <c r="F24" s="119"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="112" t="s">
         <v>555</v>
       </c>
@@ -11728,7 +11738,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="112" t="s">
         <v>556</v>
       </c>
@@ -11746,7 +11756,7 @@
       </c>
       <c r="F26" s="119"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="112" t="s">
         <v>557</v>
       </c>
@@ -11762,7 +11772,7 @@
       <c r="E27" s="105"/>
       <c r="F27" s="119"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="112" t="s">
         <v>558</v>
       </c>
@@ -11778,7 +11788,7 @@
       <c r="E28" s="105"/>
       <c r="F28" s="119"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="112" t="s">
         <v>559</v>
       </c>
@@ -11812,7 +11822,7 @@
       <c r="E30" s="105"/>
       <c r="F30" s="119"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="112" t="s">
         <v>561</v>
       </c>
@@ -11830,7 +11840,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="112" t="s">
         <v>562</v>
       </c>
@@ -11846,7 +11856,7 @@
       <c r="E32" s="105"/>
       <c r="F32" s="119"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="112" t="s">
         <v>563</v>
       </c>
@@ -11882,7 +11892,7 @@
       <c r="E34" s="105"/>
       <c r="F34" s="119"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="112" t="s">
         <v>565</v>
       </c>
@@ -11916,7 +11926,7 @@
       </c>
       <c r="F36" s="119"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="112" t="s">
         <v>567</v>
       </c>
@@ -11932,7 +11942,7 @@
       <c r="E37" s="105"/>
       <c r="F37" s="119"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="112" t="s">
         <v>568</v>
       </c>
@@ -11948,7 +11958,7 @@
       <c r="E38" s="105"/>
       <c r="F38" s="119"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="112" t="s">
         <v>569</v>
       </c>
@@ -11964,7 +11974,7 @@
       <c r="E39" s="105"/>
       <c r="F39" s="119"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="112" t="s">
         <v>570</v>
       </c>
@@ -11992,13 +12002,15 @@
       <c r="C41" s="116" t="s">
         <v>373</v>
       </c>
-      <c r="D41" s="104" t="s">
-        <v>111</v>
-      </c>
-      <c r="E41" s="105"/>
+      <c r="D41" s="123" t="s">
+        <v>327</v>
+      </c>
+      <c r="E41" s="105" t="s">
+        <v>632</v>
+      </c>
       <c r="F41" s="119"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="112" t="s">
         <v>572</v>
       </c>
@@ -12016,7 +12028,7 @@
       </c>
       <c r="F42" s="119"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="112" t="s">
         <v>573</v>
       </c>
@@ -12032,7 +12044,7 @@
       <c r="E43" s="105"/>
       <c r="F43" s="119"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="112" t="s">
         <v>574</v>
       </c>
@@ -12050,7 +12062,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="112" t="s">
         <v>575</v>
       </c>
@@ -12068,7 +12080,7 @@
       </c>
       <c r="F45" s="119"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="112" t="s">
         <v>576</v>
       </c>
@@ -12102,7 +12114,7 @@
       <c r="E47" s="105"/>
       <c r="F47" s="119"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="112" t="s">
         <v>578</v>
       </c>
@@ -12118,7 +12130,7 @@
       <c r="E48" s="105"/>
       <c r="F48" s="119"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="112" t="s">
         <v>579</v>
       </c>
@@ -12134,7 +12146,7 @@
       <c r="E49" s="105"/>
       <c r="F49" s="119"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="112" t="s">
         <v>580</v>
       </c>
@@ -12152,7 +12164,7 @@
       </c>
       <c r="F50" s="119"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="112" t="s">
         <v>581</v>
       </c>
@@ -12170,7 +12182,7 @@
       </c>
       <c r="F51" s="119"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="112" t="s">
         <v>582</v>
       </c>
@@ -12188,7 +12200,7 @@
       </c>
       <c r="F52" s="119"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="112" t="s">
         <v>583</v>
       </c>
@@ -12204,7 +12216,7 @@
       <c r="E53" s="105"/>
       <c r="F53" s="119"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="112" t="s">
         <v>584</v>
       </c>
@@ -12220,7 +12232,7 @@
       <c r="E54" s="105"/>
       <c r="F54" s="119"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="112" t="s">
         <v>585</v>
       </c>
@@ -12238,7 +12250,7 @@
       </c>
       <c r="F55" s="119"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="112" t="s">
         <v>586</v>
       </c>
@@ -12256,7 +12268,7 @@
       </c>
       <c r="F56" s="119"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="112" t="s">
         <v>598</v>
       </c>
@@ -12272,7 +12284,7 @@
       <c r="E57" s="105"/>
       <c r="F57" s="119"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="112" t="s">
         <v>600</v>
       </c>
@@ -12288,7 +12300,7 @@
       <c r="E58" s="105"/>
       <c r="F58" s="119"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="112" t="s">
         <v>602</v>
       </c>
@@ -12323,11 +12335,21 @@
       <c r="F60" s="119"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F60">
+    <filterColumn colId="0" showButton="0"/>
+    <filterColumn colId="1" showButton="0"/>
+    <filterColumn colId="2" showButton="0">
+      <filters>
+        <filter val="Luis Miguel"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:D2"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>